<commit_message>
Movie site HTML semantics finished
</commit_message>
<xml_diff>
--- a/week-4/homework/dmmawcoe-medialist.xlsx
+++ b/week-4/homework/dmmawcoe-medialist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmmco\Desktop\College Stuff\IST 263\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmmco\Desktop\Everything\College Stuff\IST 263\ist263\week-4\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B548AF-805A-4540-967D-3FBF0774A558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E9BCCD-0213-4517-BAB3-0D28ACFA7F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C261A29B-8E6B-410D-976E-B0FA0E4E92CD}"/>
+    <workbookView xWindow="3195" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{C261A29B-8E6B-410D-976E-B0FA0E4E92CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Filename</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>More to add… just want to make sure my lists are solid before doing so</t>
+  </si>
+  <si>
+    <t>Pulp Fiction Poster</t>
   </si>
 </sst>
 </file>
@@ -263,6 +266,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -281,18 +296,6 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -307,13 +310,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F739E1E-1C13-46CB-9987-E27171D49D40}" name="Table2" displayName="Table2" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F739E1E-1C13-46CB-9987-E27171D49D40}" name="Table2" displayName="Table2" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D1048576" xr:uid="{F13648D9-8A3B-49CA-BB02-1FA2C30EE2F0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5C9E26C2-7F86-4C97-BABB-AE1D8D3AF564}" name="Filename" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B5120F1E-1E5C-400B-A621-D5551ECF81BA}" name="Source" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{21C2C875-5C58-4E42-9D34-A0AA94866ECF}" name="Owner" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{F71285AD-1EBA-4C9A-B672-E1180F224C63}" name="Licensed for Reuse" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5C9E26C2-7F86-4C97-BABB-AE1D8D3AF564}" name="Filename" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B5120F1E-1E5C-400B-A621-D5551ECF81BA}" name="Source" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{21C2C875-5C58-4E42-9D34-A0AA94866ECF}" name="Owner" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F71285AD-1EBA-4C9A-B672-E1180F224C63}" name="Licensed for Reuse" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -618,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21134D7E-6632-4F93-8C27-338F1B8D2FB0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,9 +664,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
-        <f>HYPERLINK("https://m.media-amazon.com/images/M/MV5BNGNhMDIzZTUtNTBlZi00MTRlLWFjM2ItYzViMjE3YzI5MjljXkEyXkFqcGdeQXVyNzkwMjQ5NzM@._V1_SY1000_CR0,0,686,1000_AL_.jpg", "Pulp Fiction Poster")</f>
-        <v>Pulp Fiction Poster</v>
+      <c r="A2" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>49</v>
@@ -888,11 +890,12 @@
     <hyperlink ref="A9" r:id="rId6" xr:uid="{6390AB21-4366-4496-A376-C745F0474AAF}"/>
     <hyperlink ref="A10" r:id="rId7" xr:uid="{B1C6C221-B1EA-4663-ADA5-F7EED89C3C01}"/>
     <hyperlink ref="A11" r:id="rId8" xr:uid="{BEC2C6CC-2B45-4958-A95F-E617B4E92A1E}"/>
+    <hyperlink ref="A2" r:id="rId9" xr:uid="{313C8EAE-821A-48FF-B2C8-39EC75440810}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added media to the sites
</commit_message>
<xml_diff>
--- a/week-4/homework/dmmawcoe-medialist.xlsx
+++ b/week-4/homework/dmmawcoe-medialist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmmco\Desktop\Everything\College Stuff\IST 263\ist263\week-4\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E9BCCD-0213-4517-BAB3-0D28ACFA7F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522A0F38-E05C-413D-AEFC-DFB5A1D87B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3195" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{C261A29B-8E6B-410D-976E-B0FA0E4E92CD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Filename</t>
   </si>
@@ -99,9 +99,6 @@
     <t>4) Forrest Gump</t>
   </si>
   <si>
-    <t>1) Djanko Unchained</t>
-  </si>
-  <si>
     <t>5) Bryan Cranston</t>
   </si>
   <si>
@@ -186,10 +183,55 @@
     <t>All sources hyperlinked to the filenames</t>
   </si>
   <si>
-    <t>More to add… just want to make sure my lists are solid before doing so</t>
-  </si>
-  <si>
     <t>Pulp Fiction Poster</t>
+  </si>
+  <si>
+    <t>1) Django Unchained</t>
+  </si>
+  <si>
+    <t>Django Unchained Trailer</t>
+  </si>
+  <si>
+    <t>YouTube - Movieclips Trailers</t>
+  </si>
+  <si>
+    <t>Taxi Driver Trailer</t>
+  </si>
+  <si>
+    <t>YouTube - Sony Pictures Home Entertainment</t>
+  </si>
+  <si>
+    <t>Clockwork Orange Trailer</t>
+  </si>
+  <si>
+    <t>American History X Trailer</t>
+  </si>
+  <si>
+    <t>YouTube - Warner Bros. Entertainment</t>
+  </si>
+  <si>
+    <t>YouTube - Movieclips Classic Trailers</t>
+  </si>
+  <si>
+    <t>Full Metal Jacket Trailer</t>
+  </si>
+  <si>
+    <t>YouTube - SuperSubject20</t>
+  </si>
+  <si>
+    <t>Rick and Morty Poster</t>
+  </si>
+  <si>
+    <t>Breaking Bad Poster</t>
+  </si>
+  <si>
+    <t>Avatar: The Last Airbender Poster</t>
+  </si>
+  <si>
+    <t>Lie To Me Poster</t>
+  </si>
+  <si>
+    <t>Letterkenny Poster</t>
   </si>
 </sst>
 </file>
@@ -619,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21134D7E-6632-4F93-8C27-338F1B8D2FB0}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,16 +707,16 @@
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -683,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
@@ -696,38 +738,38 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3"/>
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>18</v>
@@ -735,80 +777,80 @@
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>13</v>
@@ -819,14 +861,14 @@
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>15</v>
@@ -837,47 +879,105 @@
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="H13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>29</v>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -891,11 +991,21 @@
     <hyperlink ref="A10" r:id="rId7" xr:uid="{B1C6C221-B1EA-4663-ADA5-F7EED89C3C01}"/>
     <hyperlink ref="A11" r:id="rId8" xr:uid="{BEC2C6CC-2B45-4958-A95F-E617B4E92A1E}"/>
     <hyperlink ref="A2" r:id="rId9" xr:uid="{313C8EAE-821A-48FF-B2C8-39EC75440810}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{DF827AF0-159D-45E0-97E2-E016A43F5756}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{EAF7C926-3DE9-44DB-B833-37886544E938}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{8CBC66E6-9AB4-444A-9BDE-A0E008B89952}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{453972E9-75DD-41A1-AE95-69E9C44A0A22}"/>
+    <hyperlink ref="A17" r:id="rId14" xr:uid="{8664F90A-417E-4127-B0BB-0F0D4BD80205}"/>
+    <hyperlink ref="A19" r:id="rId15" xr:uid="{9A71CF55-F103-4271-8BDC-9A6BE5E32A73}"/>
+    <hyperlink ref="A20" r:id="rId16" xr:uid="{9338C6F0-2E1C-47F0-AF93-BFCF7FABA55E}"/>
+    <hyperlink ref="A21" r:id="rId17" xr:uid="{A1C202A5-1605-41B0-AC70-8D3685A14D35}"/>
+    <hyperlink ref="A23" r:id="rId18" xr:uid="{F1696BC6-3C8A-44B3-A218-810E1DBD20BF}"/>
+    <hyperlink ref="A22" r:id="rId19" xr:uid="{6404B8CB-A960-4A54-98D7-E5B2858E27CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>